<commit_message>
N8 Push: 2025-03-12 18:17:59
</commit_message>
<xml_diff>
--- a/TIMESHEET/TimeSheet.xlsx
+++ b/TIMESHEET/TimeSheet.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="181">
   <si>
     <t xml:space="preserve">Intern</t>
   </si>
@@ -1738,7 +1738,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="8.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="16.38"/>
@@ -2448,7 +2448,7 @@
       <selection pane="bottomLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="34.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="34.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="29" width="34.08"/>
@@ -3286,7 +3286,7 @@
       <selection pane="bottomLeft" activeCell="N32" activeCellId="0" sqref="N32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="8.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="11.57"/>
@@ -4716,7 +4716,7 @@
       <selection pane="bottomLeft" activeCell="F29" activeCellId="0" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="9.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="32.14"/>
@@ -6122,11 +6122,11 @@
   </sheetPr>
   <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O12" activeCellId="0" sqref="O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="27.58"/>
@@ -6527,7 +6527,9 @@
       <c r="H9" s="67" t="s">
         <v>119</v>
       </c>
-      <c r="I9" s="40"/>
+      <c r="I9" s="40" t="n">
+        <v>7</v>
+      </c>
       <c r="J9" s="40"/>
       <c r="K9" s="67"/>
       <c r="L9" s="67"/>
@@ -6550,50 +6552,76 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="90" t="n">
+      <c r="A10" s="91" t="n">
         <v>45725</v>
       </c>
-      <c r="B10" s="67"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="67"/>
-      <c r="L10" s="67"/>
-      <c r="M10" s="40"/>
-      <c r="N10" s="67"/>
-      <c r="O10" s="40"/>
-      <c r="P10" s="40"/>
-      <c r="Q10" s="67"/>
-      <c r="R10" s="67"/>
-      <c r="S10" s="67"/>
+      <c r="B10" s="92" t="s">
+        <v>180</v>
+      </c>
+      <c r="C10" s="92"/>
+      <c r="D10" s="92"/>
+      <c r="E10" s="92"/>
+      <c r="F10" s="92"/>
+      <c r="G10" s="92"/>
+      <c r="H10" s="92"/>
+      <c r="I10" s="93"/>
+      <c r="J10" s="93" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" s="92"/>
+      <c r="L10" s="92"/>
+      <c r="M10" s="93"/>
+      <c r="N10" s="92"/>
+      <c r="O10" s="93"/>
+      <c r="P10" s="93"/>
+      <c r="Q10" s="92"/>
+      <c r="R10" s="92"/>
+      <c r="S10" s="92"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="90" t="n">
         <v>45726</v>
       </c>
-      <c r="B11" s="67"/>
-      <c r="C11" s="67"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="67"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="67"/>
-      <c r="I11" s="40"/>
+      <c r="B11" s="67" t="s">
+        <v>176</v>
+      </c>
+      <c r="C11" s="67" t="s">
+        <v>176</v>
+      </c>
+      <c r="D11" s="67" t="s">
+        <v>177</v>
+      </c>
+      <c r="E11" s="67" t="s">
+        <v>155</v>
+      </c>
+      <c r="F11" s="67" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="67" t="s">
+        <v>138</v>
+      </c>
+      <c r="H11" s="67" t="s">
+        <v>119</v>
+      </c>
+      <c r="I11" s="40" t="n">
+        <v>8</v>
+      </c>
       <c r="J11" s="40"/>
       <c r="K11" s="67"/>
       <c r="L11" s="67"/>
       <c r="M11" s="40"/>
       <c r="N11" s="67"/>
-      <c r="O11" s="40"/>
-      <c r="P11" s="40"/>
+      <c r="O11" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="P11" s="40" t="s">
+        <v>179</v>
+      </c>
       <c r="Q11" s="67"/>
       <c r="R11" s="67"/>
-      <c r="S11" s="67"/>
+      <c r="S11" s="67" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="90" t="n">

</xml_diff>